<commit_message>
Push Stuff in main
</commit_message>
<xml_diff>
--- a/PredictionMean.xlsx
+++ b/PredictionMean.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Materia BioWorks\Projects\materiaModelTraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463D16BE-7245-436F-9B07-B9A0C1F0F5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D944CA-452D-41E7-B1A3-79F1B597D0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4396638E-3CB6-431B-AF00-DD65AAA19B68}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{4396638E-3CB6-431B-AF00-DD65AAA19B68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -483,21 +483,21 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
     <col min="6" max="6" width="36" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -534,7 +534,7 @@
         <v>2.1556486675259401</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -551,7 +551,7 @@
         <v>78.832201216873401</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -562,7 +562,7 @@
         <v>48.820676855895201</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -573,7 +573,7 @@
         <v>4.6883136686202196</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -584,7 +584,7 @@
         <v>93.217209189238403</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -596,7 +596,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -613,7 +613,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -624,7 +624,7 @@
         <v>13.4752223266721</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -635,7 +635,7 @@
         <v>28.457034768059501</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -646,7 +646,7 @@
         <v>4.3890722049549504</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -657,7 +657,7 @@
         <v>0.25738312284482701</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -668,7 +668,7 @@
         <v>91.174237371412403</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -679,7 +679,7 @@
         <v>10.257643203834</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -696,7 +696,7 @@
         <v>0.145027160244911</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>

</xml_diff>